<commit_message>
Intervalos Nomeados e Listas Condicionadas (=INDIRETO)
</commit_message>
<xml_diff>
--- a/4-FerramentasDeDados/15. Validação de Dados - Intervalos Nomeados - Material(1).xlsx
+++ b/4-FerramentasDeDados/15. Validação de Dados - Intervalos Nomeados - Material(1).xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24228"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27932"/>
   <workbookPr hidePivotFieldList="1" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\joaof\Desktop\Excel Impressionador 2021\Módulo 7 - Ferramentas de Dados\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\workspace\cursos\excel\4-FerramentasDeDados\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D1C740BA-6949-4CBA-B312-CF1D59B75C7B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4144D47B-D773-47C5-90B2-B0D0C135201F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="1000" xr2:uid="{0D445F65-54A1-41E5-865A-2279466CCF1F}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" tabRatio="1000" activeTab="1" xr2:uid="{0D445F65-54A1-41E5-865A-2279466CCF1F}"/>
   </bookViews>
   <sheets>
     <sheet name="Base" sheetId="2" r:id="rId1"/>
@@ -19,6 +19,19 @@
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">Paises!$A$1:$E$55</definedName>
+    <definedName name="África">Paises!$A$2:$A$11</definedName>
+    <definedName name="América">Paises!$B$2:$B$11</definedName>
+    <definedName name="Ásia">Paises!$C$2:$C$11</definedName>
+    <definedName name="Continentes">Paises!$A$1:$E$1</definedName>
+    <definedName name="Equipe">Base!$H$2:$H$5</definedName>
+    <definedName name="Europa">Paises!$D$2:$D$11</definedName>
+    <definedName name="Oceania">Paises!$E$2:$E$11</definedName>
+    <definedName name="PaisesAfrica">Paises!$A$2:$A$11</definedName>
+    <definedName name="PaisesAmerica">Paises!$B$2:$B$11</definedName>
+    <definedName name="PaisesAsia">Paises!$C$2:$C$11</definedName>
+    <definedName name="PaisesEuropa">Paises!$D$2:$D$11</definedName>
+    <definedName name="PaisesOceania">Paises!$E$2:$E$11</definedName>
+    <definedName name="Sexo">Base!$J$2:$J$4</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -39,7 +52,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="67">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="70">
   <si>
     <t>Nome</t>
   </si>
@@ -240,6 +253,15 @@
   </si>
   <si>
     <t>País</t>
+  </si>
+  <si>
+    <t>Masculino</t>
+  </si>
+  <si>
+    <t>Feminino</t>
+  </si>
+  <si>
+    <t>Outros</t>
   </si>
 </sst>
 </file>
@@ -265,7 +287,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="6">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -293,6 +315,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="0" tint="-4.9989318521683403E-2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -324,7 +352,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
@@ -339,6 +367,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -357,9 +386,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema do Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema do Office 2013 - 2022">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -397,7 +426,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -503,7 +532,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -645,7 +674,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -653,19 +682,21 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{40D11AF4-2C8D-4548-9F11-4E03C4C35DE5}">
-  <dimension ref="A1:I7089"/>
+  <dimension ref="A1:J7089"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0"/>
+    <sheetView showGridLines="0" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="C3" sqref="C3"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="21.5546875" customWidth="1"/>
-    <col min="2" max="6" width="19.21875" customWidth="1"/>
-    <col min="8" max="8" width="12.44140625" customWidth="1"/>
-    <col min="9" max="9" width="8.88671875" style="4"/>
+    <col min="1" max="1" width="21.5703125" customWidth="1"/>
+    <col min="2" max="6" width="19.28515625" customWidth="1"/>
+    <col min="8" max="8" width="12.42578125" customWidth="1"/>
+    <col min="9" max="9" width="8.85546875" style="4"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A1" s="9" t="s">
         <v>0</v>
       </c>
@@ -687,8 +718,11 @@
       <c r="H1" s="3" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="J1" s="12" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2" s="10"/>
       <c r="B2" s="5"/>
       <c r="C2" s="5"/>
@@ -698,30 +732,40 @@
       <c r="H2" s="2" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="J2" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3" s="11"/>
       <c r="B3" s="5"/>
       <c r="C3" s="5"/>
       <c r="D3" s="5"/>
-      <c r="E3" s="5"/>
       <c r="F3" s="5"/>
       <c r="H3" s="2" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="J3" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4" s="5"/>
       <c r="B4" s="5"/>
-      <c r="C4" s="5"/>
+      <c r="C4" s="5" t="s">
+        <v>67</v>
+      </c>
       <c r="D4" s="5"/>
       <c r="E4" s="5"/>
       <c r="F4" s="5"/>
       <c r="H4" s="2" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="J4" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5" s="5"/>
       <c r="B5" s="5"/>
       <c r="C5" s="5"/>
@@ -732,7 +776,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A6" s="5"/>
       <c r="B6" s="5"/>
       <c r="C6" s="5"/>
@@ -740,7 +784,7 @@
       <c r="E6" s="5"/>
       <c r="F6" s="5"/>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A7" s="5"/>
       <c r="B7" s="5"/>
       <c r="C7" s="5"/>
@@ -748,7 +792,7 @@
       <c r="E7" s="5"/>
       <c r="F7" s="5"/>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A8" s="5"/>
       <c r="B8" s="5"/>
       <c r="C8" s="5"/>
@@ -756,7 +800,7 @@
       <c r="E8" s="5"/>
       <c r="F8" s="5"/>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A9" s="5"/>
       <c r="B9" s="5"/>
       <c r="C9" s="5"/>
@@ -764,7 +808,7 @@
       <c r="E9" s="5"/>
       <c r="F9" s="5"/>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A10" s="5"/>
       <c r="B10" s="5"/>
       <c r="C10" s="5"/>
@@ -772,7 +816,7 @@
       <c r="E10" s="5"/>
       <c r="F10" s="5"/>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A11" s="5"/>
       <c r="B11" s="5"/>
       <c r="C11" s="5"/>
@@ -780,7 +824,7 @@
       <c r="E11" s="5"/>
       <c r="F11" s="5"/>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A12" s="5"/>
       <c r="B12" s="5"/>
       <c r="C12" s="5"/>
@@ -788,7 +832,7 @@
       <c r="E12" s="5"/>
       <c r="F12" s="5"/>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A13" s="5"/>
       <c r="B13" s="5"/>
       <c r="C13" s="5"/>
@@ -796,7 +840,7 @@
       <c r="E13" s="5"/>
       <c r="F13" s="5"/>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A14" s="5"/>
       <c r="B14" s="5"/>
       <c r="C14" s="5"/>
@@ -804,7 +848,7 @@
       <c r="E14" s="5"/>
       <c r="F14" s="5"/>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A15" s="5"/>
       <c r="B15" s="5"/>
       <c r="C15" s="5"/>
@@ -812,10 +856,18 @@
       <c r="E15" s="5"/>
       <c r="F15" s="5"/>
     </row>
-    <row r="7089" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="7089" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A7089" s="1"/>
     </row>
   </sheetData>
+  <dataValidations count="2">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B2" xr:uid="{199FBC84-B26A-4B5D-ABA4-618782F98647}">
+      <formula1>Equipe</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C4" xr:uid="{AD9919FD-1459-4A7A-94C7-5782C6787FE9}">
+      <formula1>Sexo</formula1>
+    </dataValidation>
+  </dataValidations>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
@@ -825,14 +877,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5F53E3B8-6343-4ACB-9A1F-E8EA93C2EABE}">
   <dimension ref="A1:E31"/>
   <sheetViews>
-    <sheetView showGridLines="0" zoomScale="120" zoomScaleNormal="120" workbookViewId="0"/>
+    <sheetView showGridLines="0" tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="E2" sqref="E2:E11"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="5" width="21.21875" customWidth="1"/>
+    <col min="1" max="5" width="21.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="7" t="s">
         <v>10</v>
       </c>
@@ -849,7 +903,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="8" t="s">
         <v>26</v>
       </c>
@@ -866,7 +920,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="8" t="s">
         <v>38</v>
       </c>
@@ -883,7 +937,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" s="8" t="s">
         <v>42</v>
       </c>
@@ -900,7 +954,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" s="8" t="s">
         <v>49</v>
       </c>
@@ -917,7 +971,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" s="8" t="s">
         <v>51</v>
       </c>
@@ -934,7 +988,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" s="8" t="s">
         <v>56</v>
       </c>
@@ -951,7 +1005,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" s="8" t="s">
         <v>58</v>
       </c>
@@ -968,7 +1022,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" s="8" t="s">
         <v>60</v>
       </c>
@@ -985,7 +1039,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" s="8" t="s">
         <v>63</v>
       </c>
@@ -1002,7 +1056,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" s="8" t="s">
         <v>64</v>
       </c>
@@ -1019,103 +1073,103 @@
         <v>35</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" s="4"/>
       <c r="B12" s="4"/>
       <c r="C12" s="4"/>
       <c r="D12" s="4"/>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" s="4"/>
       <c r="B13" s="4"/>
       <c r="C13" s="4"/>
       <c r="D13" s="4"/>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" s="4"/>
       <c r="B14" s="4"/>
       <c r="C14" s="4"/>
       <c r="D14" s="4"/>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15" s="4"/>
       <c r="B15" s="4"/>
       <c r="C15" s="4"/>
       <c r="D15" s="4"/>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16" s="4"/>
       <c r="B16" s="4"/>
       <c r="C16" s="4"/>
       <c r="D16" s="4"/>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17" s="4"/>
       <c r="B17" s="4"/>
       <c r="C17" s="4"/>
       <c r="D17" s="4"/>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18" s="4"/>
       <c r="B18" s="4"/>
       <c r="C18" s="4"/>
       <c r="D18" s="4"/>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19" s="4"/>
       <c r="B19" s="4"/>
       <c r="C19" s="4"/>
       <c r="D19" s="4"/>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20" s="4"/>
       <c r="B20" s="4"/>
       <c r="C20" s="4"/>
       <c r="D20" s="4"/>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A21" s="4"/>
       <c r="B21" s="4"/>
       <c r="C21" s="4"/>
       <c r="D21" s="4"/>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A22" s="4"/>
       <c r="B22" s="4"/>
       <c r="C22" s="4"/>
       <c r="D22" s="4"/>
     </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A23" s="4"/>
       <c r="B23" s="4"/>
       <c r="C23" s="4"/>
       <c r="D23" s="4"/>
     </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A24" s="4"/>
       <c r="B24" s="4"/>
       <c r="C24" s="4"/>
       <c r="D24" s="4"/>
     </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A25" s="4"/>
     </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A26" s="4"/>
     </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A27" s="4"/>
     </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A28" s="4"/>
     </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A29" s="4"/>
     </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A30" s="4"/>
     </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A31" s="4"/>
     </row>
   </sheetData>
@@ -1127,14 +1181,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A4078EFF-B788-452D-9850-73BA89964DF3}">
   <dimension ref="A1:B2"/>
   <sheetViews>
-    <sheetView showGridLines="0" zoomScale="120" zoomScaleNormal="120" workbookViewId="0"/>
+    <sheetView showGridLines="0" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="2" width="30.21875" customWidth="1"/>
+    <col min="1" max="2" width="30.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="6" t="s">
         <v>65</v>
       </c>
@@ -1142,11 +1198,21 @@
         <v>66</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A2" s="5"/>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" s="5" t="s">
+        <v>13</v>
+      </c>
       <c r="B2" s="5"/>
     </row>
   </sheetData>
+  <dataValidations count="2">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A2" xr:uid="{E0BECD7F-36E3-431F-823B-12AB7223E4D3}">
+      <formula1>Continentes</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B2" xr:uid="{F7FFAEA7-433C-463B-B8BF-0916A576C04D}">
+      <formula1>INDIRECT(A2)</formula1>
+    </dataValidation>
+  </dataValidations>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Invervalos Nomeados e Listas Condicionais(=INDIRETO())
</commit_message>
<xml_diff>
--- a/4-FerramentasDeDados/15. Validação de Dados - Intervalos Nomeados - Material(1).xlsx
+++ b/4-FerramentasDeDados/15. Validação de Dados - Intervalos Nomeados - Material(1).xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\workspace\cursos\excel\4-FerramentasDeDados\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4144D47B-D773-47C5-90B2-B0D0C135201F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E8A6D696-90E0-4E9A-A12A-DE9EA8A05CB7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" tabRatio="1000" activeTab="1" xr2:uid="{0D445F65-54A1-41E5-865A-2279466CCF1F}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" tabRatio="1000" activeTab="2" xr2:uid="{0D445F65-54A1-41E5-865A-2279466CCF1F}"/>
   </bookViews>
   <sheets>
     <sheet name="Base" sheetId="2" r:id="rId1"/>
@@ -20,15 +20,15 @@
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">Paises!$A$1:$E$55</definedName>
     <definedName name="África">Paises!$A$2:$A$11</definedName>
-    <definedName name="América">Paises!$B$2:$B$11</definedName>
-    <definedName name="Ásia">Paises!$C$2:$C$11</definedName>
+    <definedName name="América">Paises!$B$2:$B$12</definedName>
+    <definedName name="Ásia">Paises!$C$2:$C$16</definedName>
     <definedName name="Continentes">Paises!$A$1:$E$1</definedName>
     <definedName name="Equipe">Base!$H$2:$H$5</definedName>
     <definedName name="Europa">Paises!$D$2:$D$11</definedName>
     <definedName name="Oceania">Paises!$E$2:$E$11</definedName>
     <definedName name="PaisesAfrica">Paises!$A$2:$A$11</definedName>
-    <definedName name="PaisesAmerica">Paises!$B$2:$B$11</definedName>
-    <definedName name="PaisesAsia">Paises!$C$2:$C$11</definedName>
+    <definedName name="PaisesAmerica">Paises!$B$2:$B$12</definedName>
+    <definedName name="PaisesAsia">Paises!$C$2:$C$16</definedName>
     <definedName name="PaisesEuropa">Paises!$D$2:$D$11</definedName>
     <definedName name="PaisesOceania">Paises!$E$2:$E$11</definedName>
     <definedName name="Sexo">Base!$J$2:$J$4</definedName>
@@ -52,7 +52,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="70">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="71">
   <si>
     <t>Nome</t>
   </si>
@@ -262,12 +262,15 @@
   </si>
   <si>
     <t>Outros</t>
+  </si>
+  <si>
+    <t>Brasil</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr9="http://schemas.microsoft.com/office/spreadsheetml/2016/revision9" mc:Ignorable="x14ac x16r2 xr xr9">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="&quot;R$&quot;\ #,##0.00"/>
   </numFmts>
@@ -325,7 +328,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="6">
     <border>
       <left/>
       <right/>
@@ -348,18 +351,61 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -368,12 +414,297 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <dxfs count="21">
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right/>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left/>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+      </border>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
+        </patternFill>
+      </fill>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="0"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="2" tint="-0.749992370372631"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="0"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="2" tint="-0.749992370372631"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="0"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="2" tint="-0.749992370372631"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="0"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="2" tint="-0.749992370372631"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="0"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="2" tint="-0.749992370372631"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+    </dxf>
+  </dxfs>
+  <tableStyles count="1" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16">
+    <tableStyle name="Branco" pivot="0" count="0" xr9:uid="{44BB9E7C-4DC4-4925-AE63-5581F407C8DF}"/>
+  </tableStyles>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -383,6 +714,67 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{1F5EC0E8-14FC-4143-BB8C-3E62EA1D518A}" name="Tabela3" displayName="Tabela3" ref="A1:A11" totalsRowShown="0" headerRowDxfId="18" dataDxfId="19">
+  <autoFilter ref="A1:A11" xr:uid="{1F5EC0E8-14FC-4143-BB8C-3E62EA1D518A}"/>
+  <tableColumns count="1">
+    <tableColumn id="1" xr3:uid="{F57E5AAF-85B3-405B-B0AF-7FBD7F6F68D3}" name="África" dataDxfId="20"/>
+  </tableColumns>
+  <tableStyleInfo name="Branco" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{3A6FB505-CC8B-4455-9AB4-DB7577889DF8}" name="Tabela4" displayName="Tabela4" ref="B1:B12" totalsRowShown="0" headerRowDxfId="15" dataDxfId="16">
+  <autoFilter ref="B1:B12" xr:uid="{3A6FB505-CC8B-4455-9AB4-DB7577889DF8}"/>
+  <tableColumns count="1">
+    <tableColumn id="1" xr3:uid="{DDD02687-84CF-4ECD-B08F-7DBEADB10EE7}" name="América" dataDxfId="17"/>
+  </tableColumns>
+  <tableStyleInfo name="Branco" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{0642667B-BE68-46E4-87CD-F5D16F4E793B}" name="Tabela5" displayName="Tabela5" ref="C1:C16" totalsRowShown="0" headerRowDxfId="8" dataDxfId="7">
+  <autoFilter ref="C1:C16" xr:uid="{0642667B-BE68-46E4-87CD-F5D16F4E793B}"/>
+  <tableColumns count="1">
+    <tableColumn id="1" xr3:uid="{FBE2A3FC-91A6-4AA4-B3A2-A5D2F5384708}" name="Ásia" dataDxfId="6"/>
+  </tableColumns>
+  <tableStyleInfo name="Branco" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="6" xr:uid="{DF65E14C-52A5-4329-950C-C1F4F55244E3}" name="Tabela6" displayName="Tabela6" ref="D1:D11" totalsRowShown="0" headerRowDxfId="12" dataDxfId="13">
+  <autoFilter ref="D1:D11" xr:uid="{DF65E14C-52A5-4329-950C-C1F4F55244E3}"/>
+  <tableColumns count="1">
+    <tableColumn id="1" xr3:uid="{062FD534-1CD2-4377-B1A9-C80D9F3C9826}" name="Europa" dataDxfId="14"/>
+  </tableColumns>
+  <tableStyleInfo name="Branco" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="7" xr:uid="{09077D17-40DB-4098-88F3-F4D837F3FFF8}" name="Tabela7" displayName="Tabela7" ref="E1:E11" totalsRowShown="0" headerRowDxfId="9" dataDxfId="10">
+  <autoFilter ref="E1:E11" xr:uid="{09077D17-40DB-4098-88F3-F4D837F3FFF8}"/>
+  <tableColumns count="1">
+    <tableColumn id="1" xr3:uid="{CF6D18A7-5989-451A-A2A4-C43764BCE0BF}" name="Oceania" dataDxfId="11"/>
+  </tableColumns>
+  <tableStyleInfo name="Branco" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table6.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="8" xr:uid="{78CD7FBC-BCEC-4E09-9298-EF2670031F46}" name="Tabela8" displayName="Tabela8" ref="A1:B4" totalsRowShown="0" headerRowDxfId="5" headerRowBorderDxfId="3" tableBorderDxfId="4" totalsRowBorderDxfId="2">
+  <autoFilter ref="A1:B4" xr:uid="{78CD7FBC-BCEC-4E09-9298-EF2670031F46}"/>
+  <tableColumns count="2">
+    <tableColumn id="1" xr3:uid="{795E48EA-7559-4E50-B8A1-62822B5EB44B}" name="Continente" dataDxfId="1"/>
+    <tableColumn id="2" xr3:uid="{601F2FF3-9BA3-4F8B-BDDB-89F6A60845CF}" name="País" dataDxfId="0"/>
+  </tableColumns>
+  <tableStyleInfo name="Branco" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -697,33 +1089,33 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A1" s="9" t="s">
+      <c r="A1" s="8" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="9" t="s">
+      <c r="B1" s="8" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="9" t="s">
+      <c r="C1" s="8" t="s">
         <v>6</v>
       </c>
-      <c r="D1" s="9" t="s">
+      <c r="D1" s="8" t="s">
         <v>7</v>
       </c>
-      <c r="E1" s="9" t="s">
+      <c r="E1" s="8" t="s">
         <v>8</v>
       </c>
-      <c r="F1" s="9" t="s">
+      <c r="F1" s="8" t="s">
         <v>9</v>
       </c>
       <c r="H1" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="J1" s="12" t="s">
+      <c r="J1" s="11" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A2" s="10"/>
+      <c r="A2" s="9"/>
       <c r="B2" s="5"/>
       <c r="C2" s="5"/>
       <c r="D2" s="5"/>
@@ -737,7 +1129,7 @@
       </c>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A3" s="11"/>
+      <c r="A3" s="10"/>
       <c r="B3" s="5"/>
       <c r="C3" s="5"/>
       <c r="D3" s="5"/>
@@ -877,8 +1269,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5F53E3B8-6343-4ACB-9A1F-E8EA93C2EABE}">
   <dimension ref="A1:E31"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="E2" sqref="E2:E11"/>
+    <sheetView showGridLines="0" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="D15" sqref="D15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -887,220 +1279,222 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A1" s="7" t="s">
+      <c r="A1" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="B1" s="7" t="s">
+      <c r="B1" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="C1" s="7" t="s">
+      <c r="C1" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="D1" s="7" t="s">
+      <c r="D1" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="E1" s="7" t="s">
+      <c r="E1" s="6" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A2" s="8" t="s">
+      <c r="A2" s="7" t="s">
         <v>26</v>
       </c>
-      <c r="B2" s="8" t="s">
+      <c r="B2" s="7" t="s">
         <v>27</v>
       </c>
-      <c r="C2" s="8" t="s">
+      <c r="C2" s="7" t="s">
         <v>43</v>
       </c>
-      <c r="D2" s="8" t="s">
+      <c r="D2" s="7" t="s">
         <v>59</v>
       </c>
-      <c r="E2" s="8" t="s">
+      <c r="E2" s="7" t="s">
         <v>28</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A3" s="8" t="s">
+      <c r="A3" s="7" t="s">
         <v>38</v>
       </c>
-      <c r="B3" s="8" t="s">
+      <c r="B3" s="7" t="s">
         <v>19</v>
       </c>
-      <c r="C3" s="8" t="s">
+      <c r="C3" s="7" t="s">
         <v>20</v>
       </c>
-      <c r="D3" s="8" t="s">
+      <c r="D3" s="7" t="s">
         <v>30</v>
       </c>
-      <c r="E3" s="8" t="s">
+      <c r="E3" s="7" t="s">
         <v>39</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A4" s="8" t="s">
+      <c r="A4" s="7" t="s">
         <v>42</v>
       </c>
-      <c r="B4" s="8" t="s">
+      <c r="B4" s="7" t="s">
         <v>32</v>
       </c>
-      <c r="C4" s="8" t="s">
+      <c r="C4" s="7" t="s">
         <v>29</v>
       </c>
-      <c r="D4" s="8" t="s">
+      <c r="D4" s="7" t="s">
         <v>24</v>
       </c>
-      <c r="E4" s="8" t="s">
+      <c r="E4" s="7" t="s">
         <v>21</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A5" s="8" t="s">
+      <c r="A5" s="7" t="s">
         <v>49</v>
       </c>
-      <c r="B5" s="8" t="s">
+      <c r="B5" s="7" t="s">
         <v>44</v>
       </c>
-      <c r="C5" s="8" t="s">
+      <c r="C5" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="D5" s="8" t="s">
+      <c r="D5" s="7" t="s">
         <v>45</v>
       </c>
-      <c r="E5" s="8" t="s">
+      <c r="E5" s="7" t="s">
         <v>33</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A6" s="8" t="s">
+      <c r="A6" s="7" t="s">
         <v>51</v>
       </c>
-      <c r="B6" s="8" t="s">
+      <c r="B6" s="7" t="s">
         <v>47</v>
       </c>
-      <c r="C6" s="8" t="s">
+      <c r="C6" s="7" t="s">
         <v>36</v>
       </c>
-      <c r="D6" s="8" t="s">
+      <c r="D6" s="7" t="s">
         <v>48</v>
       </c>
-      <c r="E6" s="8" t="s">
+      <c r="E6" s="7" t="s">
         <v>31</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A7" s="8" t="s">
+      <c r="A7" s="7" t="s">
         <v>56</v>
       </c>
-      <c r="B7" s="8" t="s">
+      <c r="B7" s="7" t="s">
         <v>53</v>
       </c>
-      <c r="C7" s="8" t="s">
+      <c r="C7" s="7" t="s">
         <v>34</v>
       </c>
-      <c r="D7" s="8" t="s">
+      <c r="D7" s="7" t="s">
         <v>54</v>
       </c>
-      <c r="E7" s="8" t="s">
+      <c r="E7" s="7" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A8" s="8" t="s">
+      <c r="A8" s="7" t="s">
         <v>58</v>
       </c>
-      <c r="B8" s="8" t="s">
+      <c r="B8" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="C8" s="8" t="s">
+      <c r="C8" s="7" t="s">
         <v>50</v>
       </c>
-      <c r="D8" s="8" t="s">
+      <c r="D8" s="7" t="s">
         <v>37</v>
       </c>
-      <c r="E8" s="8" t="s">
+      <c r="E8" s="7" t="s">
         <v>25</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A9" s="8" t="s">
+      <c r="A9" s="7" t="s">
         <v>60</v>
       </c>
-      <c r="B9" s="8" t="s">
+      <c r="B9" s="7" t="s">
         <v>41</v>
       </c>
-      <c r="C9" s="8" t="s">
+      <c r="C9" s="7" t="s">
         <v>52</v>
       </c>
-      <c r="D9" s="8" t="s">
+      <c r="D9" s="7" t="s">
         <v>18</v>
       </c>
-      <c r="E9" s="8" t="s">
+      <c r="E9" s="7" t="s">
         <v>22</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A10" s="8" t="s">
+      <c r="A10" s="7" t="s">
         <v>63</v>
       </c>
-      <c r="B10" s="8" t="s">
+      <c r="B10" s="7" t="s">
         <v>46</v>
       </c>
-      <c r="C10" s="8" t="s">
+      <c r="C10" s="7" t="s">
         <v>57</v>
       </c>
-      <c r="D10" s="8" t="s">
+      <c r="D10" s="7" t="s">
         <v>40</v>
       </c>
-      <c r="E10" s="8" t="s">
+      <c r="E10" s="7" t="s">
         <v>23</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A11" s="8" t="s">
+      <c r="A11" s="7" t="s">
         <v>64</v>
       </c>
-      <c r="B11" s="8" t="s">
+      <c r="B11" s="7" t="s">
         <v>55</v>
       </c>
-      <c r="C11" s="8" t="s">
+      <c r="C11" s="7" t="s">
         <v>62</v>
       </c>
-      <c r="D11" s="8" t="s">
+      <c r="D11" s="7" t="s">
         <v>61</v>
       </c>
-      <c r="E11" s="8" t="s">
+      <c r="E11" s="7" t="s">
         <v>35</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" s="4"/>
-      <c r="B12" s="4"/>
-      <c r="C12" s="4"/>
+      <c r="B12" s="7" t="s">
+        <v>70</v>
+      </c>
+      <c r="C12" s="7"/>
       <c r="D12" s="4"/>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" s="4"/>
       <c r="B13" s="4"/>
-      <c r="C13" s="4"/>
+      <c r="C13" s="7"/>
       <c r="D13" s="4"/>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" s="4"/>
       <c r="B14" s="4"/>
-      <c r="C14" s="4"/>
+      <c r="C14" s="7"/>
       <c r="D14" s="4"/>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15" s="4"/>
       <c r="B15" s="4"/>
-      <c r="C15" s="4"/>
+      <c r="C15" s="7"/>
       <c r="D15" s="4"/>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16" s="4"/>
       <c r="B16" s="4"/>
-      <c r="C16" s="4"/>
+      <c r="C16" s="7"/>
       <c r="D16" s="4"/>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
@@ -1174,15 +1568,22 @@
     </row>
   </sheetData>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+  <tableParts count="5">
+    <tablePart r:id="rId1"/>
+    <tablePart r:id="rId2"/>
+    <tablePart r:id="rId3"/>
+    <tablePart r:id="rId4"/>
+    <tablePart r:id="rId5"/>
+  </tableParts>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A4078EFF-B788-452D-9850-73BA89964DF3}">
-  <dimension ref="A1:B2"/>
+  <dimension ref="A1:B4"/>
   <sheetViews>
-    <sheetView showGridLines="0" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView showGridLines="0" tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1191,28 +1592,49 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A1" s="6" t="s">
+      <c r="A1" s="12" t="s">
         <v>65</v>
       </c>
-      <c r="B1" s="6" t="s">
+      <c r="B1" s="13" t="s">
         <v>66</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A2" s="5" t="s">
+      <c r="A2" s="14" t="s">
+        <v>11</v>
+      </c>
+      <c r="B2" s="15" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" s="14" t="s">
         <v>13</v>
       </c>
-      <c r="B2" s="5"/>
+      <c r="B3" s="15" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" s="14" t="s">
+        <v>14</v>
+      </c>
+      <c r="B4" s="15" t="s">
+        <v>33</v>
+      </c>
     </row>
   </sheetData>
   <dataValidations count="2">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A2" xr:uid="{E0BECD7F-36E3-431F-823B-12AB7223E4D3}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A2:A4" xr:uid="{E0BECD7F-36E3-431F-823B-12AB7223E4D3}">
       <formula1>Continentes</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B2" xr:uid="{F7FFAEA7-433C-463B-B8BF-0916A576C04D}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B2:B4" xr:uid="{F7FFAEA7-433C-463B-B8BF-0916A576C04D}">
       <formula1>INDIRECT(A2)</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+  <tableParts count="1">
+    <tablePart r:id="rId1"/>
+  </tableParts>
 </worksheet>
 </file>
</xml_diff>